<commit_message>
updating med results for floweringtime, cobd,and tkv
</commit_message>
<xml_diff>
--- a/data/genes_identified.xlsx
+++ b/data/genes_identified.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="gddtosilk" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="278">
   <si>
     <t>MEDFIX0.5</t>
   </si>
@@ -810,6 +810,54 @@
   </si>
   <si>
     <t>/Arabidopsis best hit: AT1G30080.1 Glycosyl hydrolase superfamily protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT1G44820.1 Peptidase M20/M25/M40 family protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT3G62240.1 RING/U-box superfamily protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT1G54500.1 Rubredoxin-like superfamily protein</t>
+  </si>
+  <si>
+    <t>tipd1 - tip growth defective1/contributes to root hair elongation and drought tolerance</t>
+  </si>
+  <si>
+    <t>hagtf6 (GNAT-transcription factor 6)/</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT2G42490.1 Copper amine oxidase family protein</t>
+  </si>
+  <si>
+    <t>Rice best hit: LOC_Os07g48244.1 ubiquinol-cytochrome c reductase complex 6.7 kDa protein putative expressed</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT2G37570.1 (SLT1) HSP20-like chaperones superfamily protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT3G03070.1 NADH-ubiquinone oxidoreductase-related</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT3G08980.1 Peptidase S24/S26A/S26B/S26C family protein</t>
+  </si>
+  <si>
+    <t>arid5 - ARID-transcription factor 5</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT3G13226.1 regulatory protein RecX family protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT3G47570.1 Leucine-rich repeat protein kinase family protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT2G36800.1 (DOGT1, UGT73C5) don-glucosyltransferase 1</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT5G03610.1 GDSL-like Lipase/Acylhydrolase superfamily protein</t>
+  </si>
+  <si>
+    <t>Arabidopsis best hit: AT2G36800.1 (DOGT1, UGT73C5) don-glucosyltransferase 1</t>
   </si>
 </sst>
 </file>
@@ -956,7 +1004,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
@@ -968,6 +1016,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1291,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2195,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2545,9 +2596,7 @@
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
@@ -2557,9 +2606,7 @@
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C62" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
@@ -3010,7 +3057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C168"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -4860,8 +4907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5296,9 +5343,7 @@
       <c r="B76" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
@@ -5470,7 +5515,9 @@
       <c r="A111" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B111" s="1"/>
+      <c r="B111" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C111" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -5493,6 +5540,9 @@
       <c r="A115" t="s">
         <v>142</v>
       </c>
+      <c r="B115" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
@@ -5514,35 +5564,47 @@
       <c r="A119" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B119" s="2"/>
+      <c r="B119" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B120" s="2"/>
+      <c r="B120" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
+      <c r="B121" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B122" s="2"/>
+      <c r="B122" s="2" t="s">
+        <v>266</v>
+      </c>
       <c r="C122" s="2"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B123" s="2"/>
+      <c r="B123" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="C123" s="2"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -5565,11 +5627,20 @@
       <c r="A127" t="s">
         <v>132</v>
       </c>
+      <c r="B127" t="s">
+        <v>265</v>
+      </c>
+      <c r="C127" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>146</v>
       </c>
+      <c r="B128" s="10" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
@@ -5619,6 +5690,9 @@
       <c r="A137" t="s">
         <v>148</v>
       </c>
+      <c r="B137" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
@@ -5637,10 +5711,12 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B142" s="6"/>
+      <c r="B142" s="5" t="s">
+        <v>270</v>
+      </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
@@ -5678,7 +5754,9 @@
       <c r="A151" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B151" s="1"/>
+      <c r="B151" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="C151" s="1"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
@@ -5698,6 +5776,9 @@
       <c r="A155" t="s">
         <v>142</v>
       </c>
+      <c r="B155" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
@@ -5719,28 +5800,36 @@
       <c r="A159" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B159" s="2"/>
+      <c r="B159" s="2" t="s">
+        <v>263</v>
+      </c>
       <c r="C159" s="2"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B160" s="2"/>
+      <c r="B160" s="2" t="s">
+        <v>265</v>
+      </c>
       <c r="C160" s="2"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B161" s="2"/>
+      <c r="B161" s="2" t="s">
+        <v>266</v>
+      </c>
       <c r="C161" s="2"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B162" s="2"/>
+      <c r="B162" s="2" t="s">
+        <v>267</v>
+      </c>
       <c r="C162" s="2"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
@@ -5763,11 +5852,17 @@
       <c r="A166" t="s">
         <v>132</v>
       </c>
+      <c r="B166" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>146</v>
       </c>
+      <c r="B167" s="10" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
@@ -5817,6 +5912,9 @@
       <c r="A176" t="s">
         <v>148</v>
       </c>
+      <c r="B176" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A179" s="6" t="s">
@@ -5838,14 +5936,18 @@
       <c r="A181" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B181" s="6"/>
+      <c r="B181" s="5" t="s">
+        <v>271</v>
+      </c>
       <c r="C181" s="6"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A182" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B182" s="6"/>
+      <c r="B182" s="5" t="s">
+        <v>272</v>
+      </c>
       <c r="C182" s="6"/>
     </row>
   </sheetData>
@@ -5858,7 +5960,7 @@
   <dimension ref="A1:C185"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6442,14 +6544,18 @@
       <c r="A112" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B112" s="1"/>
+      <c r="B112" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B113" s="1"/>
+      <c r="B113" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="C113" s="1"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -6466,11 +6572,6 @@
       </c>
       <c r="C116" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B117" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -6530,11 +6631,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B131" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>78</v>
@@ -6577,12 +6673,7 @@
         <v>171</v>
       </c>
       <c r="B139" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B140" t="s">
-        <v>73</v>
+        <v>275</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
@@ -6641,14 +6732,18 @@
       <c r="A153" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B153" s="1"/>
+      <c r="B153" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="C153" s="1"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B154" s="1"/>
+      <c r="B154" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="C154" s="1"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
@@ -6667,11 +6762,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B158" t="s">
-        <v>66</v>
-      </c>
-    </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>75</v>
@@ -6692,7 +6782,9 @@
       <c r="A162" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B162" s="2"/>
+      <c r="B162" s="2" t="s">
+        <v>276</v>
+      </c>
       <c r="C162" s="2"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
@@ -6726,11 +6818,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B171" t="s">
-        <v>69</v>
-      </c>
-    </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="4" t="s">
         <v>78</v>
@@ -6773,12 +6860,7 @@
         <v>171</v>
       </c>
       <c r="B179" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B180" t="s">
-        <v>73</v>
+        <v>277</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.35">
@@ -6809,5 +6891,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>